<commit_message>
Faker added on certain area of user and vendor dashboard. Thread sleep replaced by wait.
</commit_message>
<xml_diff>
--- a/YBtestCredentials.xlsx
+++ b/YBtestCredentials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\YarsaBazar_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8CC1A0-1EA7-413F-9A71-0599573EAB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04272A13-11E8-4B6C-9E03-DF0B157AB86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{32694C23-CC6C-486E-8E8D-75DA86E9D6CD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{32694C23-CC6C-486E-8E8D-75DA86E9D6CD}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>s</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>Bloom Bee</t>
-  </si>
-  <si>
-    <t>bee@gmail.com</t>
   </si>
   <si>
     <t>phone number</t>
@@ -247,6 +244,12 @@
   </si>
   <si>
     <t>Saffron</t>
+  </si>
+  <si>
+    <t>bee1@gmail.com</t>
+  </si>
+  <si>
+    <t>9772..552113</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752A03D1-88B2-4373-928C-923D3EE45E01}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -640,10 +643,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -778,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15E5658-B766-4888-8A40-13F9E501AD0A}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -809,10 +812,10 @@
         <v>50</v>
       </c>
       <c r="B2">
-        <v>9803321453</v>
+        <v>9800321453</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
@@ -823,7 +826,7 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>9825874166</v>
+        <v>9.825088978687871E+18</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -903,8 +906,8 @@
       <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9">
-        <v>9772552113</v>
+      <c r="B9" t="s">
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -1038,36 +1041,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3">
         <v>9823579453</v>
       </c>
       <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>60</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1091,10 +1094,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1102,7 +1105,7 @@
         <v>9823579453</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1132,36 +1135,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>67</v>
       </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
       <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>9783654273</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2">
         <v>18</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel sheet combined for sign up and loging at one sheet as well as combined request for quote and RFD combined at one sheet.
</commit_message>
<xml_diff>
--- a/YBtestCredentials.xlsx
+++ b/YBtestCredentials.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\YarsaBazar_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F9DE2F-A302-46D5-A7D3-4733DCE9541C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706FD358-E798-4125-A448-BB70A79B69C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{32694C23-CC6C-486E-8E8D-75DA86E9D6CD}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{32694C23-CC6C-486E-8E8D-75DA86E9D6CD}"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="sign up" sheetId="2" r:id="rId2"/>
-    <sheet name="request for data" sheetId="4" r:id="rId3"/>
-    <sheet name="vendor login" sheetId="5" r:id="rId4"/>
-    <sheet name="RFQ" sheetId="6" r:id="rId5"/>
+    <sheet name="sign up and login" sheetId="2" r:id="rId1"/>
+    <sheet name="RFD and RFQ" sheetId="4" r:id="rId2"/>
+    <sheet name="vendor login" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t>s</t>
   </si>
@@ -55,9 +53,6 @@
     <t>%3%LKBCvJ^</t>
   </si>
   <si>
-    <t>$2a$04$O6JWaIFCZl3/Ay6GTY9nteDrxXlfgjZSwUT/pu8v7..L2jFpptFvi</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -226,23 +221,6 @@
     <t>Rquantity</t>
   </si>
   <si>
-    <t>Rdesc</t>
-  </si>
-  <si>
-    <t>Rfullname</t>
-  </si>
-  <si>
-    <t>Rmobile</t>
-  </si>
-  <si>
-    <t>Sabina Bajra</t>
-  </si>
-  <si>
-    <t>Your perfect bouquet is fresh and free from any 
-browned edges. Pick up several bouquets from 
-the selection you're presented with and inspect.</t>
-  </si>
-  <si>
     <t>Saffron</t>
   </si>
   <si>
@@ -250,6 +228,9 @@
   </si>
   <si>
     <t>9772..552113</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $2a$04$tWjqxWjUYap9wozZTK2qbkEMAa6sYEXl/ZyavuZk.</t>
   </si>
 </sst>
 </file>
@@ -300,18 +281,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -628,161 +614,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{752A03D1-88B2-4373-928C-923D3EE45E01}">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15E5658-B766-4888-8A40-13F9E501AD0A}">
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.26953125" customWidth="1"/>
-    <col min="2" max="2" width="76.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>9762784654</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>9233775446</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>3289803370</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>8179960820</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>9274210705</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>276458227</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>5804349844</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>4781440808</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>9565223436</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>1667678975</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>6864291128</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
-        <v>7561030268</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>2718114383</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
-        <v>8896886236</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>9274210705</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{97E9B652-9832-4305-86EC-953E779AF211}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15E5658-B766-4888-8A40-13F9E501AD0A}">
-  <dimension ref="A1:D16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -795,41 +631,41 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2">
         <v>9800321453</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>9.825088978687871E+18</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3">
-        <v>9.825088978687871E+18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -837,13 +673,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>99665726307</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4">
-        <v>99665726307</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -851,13 +687,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1234569808</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5">
-        <v>1234569808</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -865,13 +701,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9800000000</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6">
-        <v>9800000000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -879,9 +715,9 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2">
         <v>9652915006</v>
       </c>
       <c r="D7" t="s">
@@ -890,13 +726,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2">
+        <v>977258888</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8">
-        <v>977258888</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -904,13 +740,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
       </c>
       <c r="D9" t="e">
         <v>#NAME?</v>
@@ -918,116 +754,149 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
         <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2">
         <v>977258888</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="2">
+        <v>9762784654</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="2">
+        <v>9233775446</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="3">
+        <v>3289803370</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="3">
+        <v>8179960820</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{CB6E1160-C0B5-40AB-B720-0C8D3B70B372}"/>
+    <hyperlink ref="D17" r:id="rId2" xr:uid="{0758AFC5-77BE-43F0-8717-99D5EED02008}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E110696A-D37D-4142-8DCC-529325A9CF2F}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1037,48 +906,65 @@
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="23.453125" customWidth="1"/>
     <col min="5" max="5" width="31.81640625" customWidth="1"/>
+    <col min="6" max="6" width="27.81640625" customWidth="1"/>
+    <col min="7" max="7" width="29.1796875" customWidth="1"/>
+    <col min="8" max="8" width="28.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="5">
+        <v>9823579453</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="3">
-        <v>9823579453</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
+      <c r="F2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="4">
+        <v>18</v>
+      </c>
+      <c r="H2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683B3F57-5C2F-4A67-8F4C-9EB0E7C00560}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1094,18 +980,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>9823579453</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1114,60 +1000,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6815A555-33C6-4B6F-B933-C7595513BA75}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.90625" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" customWidth="1"/>
-    <col min="4" max="4" width="24.6328125" customWidth="1"/>
-    <col min="5" max="5" width="42.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2">
-        <v>9783654273</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2">
-        <v>18</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>